<commit_message>
updated synthetic data quality framework table
</commit_message>
<xml_diff>
--- a/LiteratureReviews/SyntheticDataQualityFrameworks/FrameworksSyntheticDataEvaluation.xlsx
+++ b/LiteratureReviews/SyntheticDataQualityFrameworks/FrameworksSyntheticDataEvaluation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://universitaetstgallen-my.sharepoint.com/personal/fabian_karst_unisg_ch/Documents/03_PhD/Research/3_ArtificialDatabaseCombination/InformationSystemResearch2024/Appendix/LiteratureReviews/SyntheticDataQualityFrameworks/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="625" documentId="8_{23A40E8C-0892-F64E-955E-9E26E389C8DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{839ED389-1D95-9C43-860A-29FCCD8ECBB8}"/>
+  <xr:revisionPtr revIDLastSave="639" documentId="8_{23A40E8C-0892-F64E-955E-9E26E389C8DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{803EB6DD-1EAC-734A-AF15-C803FE5EF01F}"/>
   <bookViews>
     <workbookView xWindow="-4860" yWindow="-21000" windowWidth="38400" windowHeight="21000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1857" uniqueCount="895">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1857" uniqueCount="909">
   <si>
     <t>Search String</t>
   </si>
@@ -2801,6 +2801,48 @@
   </si>
   <si>
     <t>Höllig &amp; Geierhos 2025</t>
+  </si>
+  <si>
+    <t>Stenger et al. 2024</t>
+  </si>
+  <si>
+    <t>Budu et al. 2023</t>
+  </si>
+  <si>
+    <t>Quian et al. 2023</t>
+  </si>
+  <si>
+    <t>Sattarov et al. 2023</t>
+  </si>
+  <si>
+    <t>Wolf et al. 2024</t>
+  </si>
+  <si>
+    <t>Simonovsky et al. 2018</t>
+  </si>
+  <si>
+    <t>Hernandez et al. 2025</t>
+  </si>
+  <si>
+    <t>Xu et al. 2021</t>
+  </si>
+  <si>
+    <t>Liu et al. 2024</t>
+  </si>
+  <si>
+    <t>Elliker et al. 2024</t>
+  </si>
+  <si>
+    <t>Sivaroopan et al. 2023</t>
+  </si>
+  <si>
+    <t>Pandey et al. 2023</t>
+  </si>
+  <si>
+    <t>Lamp et al. 2023</t>
+  </si>
+  <si>
+    <t>Yu &amp; Karray 2022</t>
   </si>
 </sst>
 </file>
@@ -3078,6 +3120,9 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -3086,9 +3131,6 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -4383,7 +4425,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" sqref="A1:AF8"/>
+      <selection pane="topRight" activeCell="X23" sqref="X23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4446,46 +4488,46 @@
         <v>894</v>
       </c>
       <c r="R1" s="33" t="s">
-        <v>40</v>
+        <v>895</v>
       </c>
       <c r="S1" s="33" t="s">
-        <v>41</v>
+        <v>896</v>
       </c>
       <c r="T1" s="33" t="s">
-        <v>42</v>
+        <v>897</v>
       </c>
       <c r="U1" s="33" t="s">
-        <v>43</v>
+        <v>898</v>
       </c>
       <c r="V1" s="33" t="s">
-        <v>44</v>
+        <v>899</v>
       </c>
       <c r="W1" s="34" t="s">
-        <v>45</v>
+        <v>900</v>
       </c>
       <c r="X1" s="34" t="s">
-        <v>46</v>
+        <v>901</v>
       </c>
       <c r="Y1" s="34" t="s">
-        <v>47</v>
+        <v>902</v>
       </c>
       <c r="Z1" s="34" t="s">
-        <v>48</v>
+        <v>903</v>
       </c>
       <c r="AA1" s="34" t="s">
-        <v>49</v>
+        <v>904</v>
       </c>
       <c r="AB1" s="34" t="s">
-        <v>50</v>
+        <v>905</v>
       </c>
       <c r="AC1" s="34" t="s">
-        <v>51</v>
+        <v>906</v>
       </c>
       <c r="AD1" s="34" t="s">
-        <v>52</v>
+        <v>907</v>
       </c>
       <c r="AE1" s="34" t="s">
-        <v>53</v>
+        <v>908</v>
       </c>
       <c r="AF1" s="24" t="s">
         <v>54</v>
@@ -4515,7 +4557,7 @@
       <c r="O2" s="15"/>
       <c r="P2" s="15"/>
       <c r="Q2" s="15"/>
-      <c r="R2" s="40" t="s">
+      <c r="R2" s="37" t="s">
         <v>64</v>
       </c>
       <c r="S2" s="15"/>
@@ -4534,7 +4576,7 @@
       <c r="AD2" s="7"/>
       <c r="AE2" s="7"/>
       <c r="AF2" s="24">
-        <f>COUNTIF(B2:AE2, "*x*")</f>
+        <f t="shared" ref="AF2:AF8" si="0">COUNTIF(B2:AE2, "*x*")</f>
         <v>4</v>
       </c>
     </row>
@@ -4552,82 +4594,82 @@
       <c r="E3" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="F3" s="40" t="s">
+      <c r="F3" s="37" t="s">
         <v>64</v>
       </c>
-      <c r="G3" s="40" t="s">
+      <c r="G3" s="37" t="s">
         <v>64</v>
       </c>
-      <c r="H3" s="40" t="s">
+      <c r="H3" s="37" t="s">
         <v>64</v>
       </c>
       <c r="I3" s="15"/>
       <c r="J3" s="35" t="s">
         <v>863</v>
       </c>
-      <c r="K3" s="40" t="s">
+      <c r="K3" s="37" t="s">
         <v>64</v>
       </c>
-      <c r="L3" s="40" t="s">
+      <c r="L3" s="37" t="s">
         <v>64</v>
       </c>
-      <c r="M3" s="40" t="s">
+      <c r="M3" s="37" t="s">
         <v>64</v>
       </c>
-      <c r="N3" s="40" t="s">
+      <c r="N3" s="37" t="s">
         <v>64</v>
       </c>
-      <c r="O3" s="40" t="s">
+      <c r="O3" s="37" t="s">
         <v>64</v>
       </c>
-      <c r="P3" s="40" t="s">
+      <c r="P3" s="37" t="s">
         <v>64</v>
       </c>
       <c r="Q3" s="15"/>
-      <c r="R3" s="40" t="s">
+      <c r="R3" s="37" t="s">
         <v>64</v>
       </c>
-      <c r="S3" s="40" t="s">
+      <c r="S3" s="37" t="s">
         <v>64</v>
       </c>
-      <c r="T3" s="40" t="s">
+      <c r="T3" s="37" t="s">
         <v>64</v>
       </c>
-      <c r="U3" s="40" t="s">
+      <c r="U3" s="37" t="s">
         <v>64</v>
       </c>
-      <c r="V3" s="40" t="s">
+      <c r="V3" s="37" t="s">
         <v>64</v>
       </c>
-      <c r="W3" s="40" t="s">
+      <c r="W3" s="37" t="s">
         <v>64</v>
       </c>
-      <c r="X3" s="40" t="s">
+      <c r="X3" s="37" t="s">
         <v>64</v>
       </c>
       <c r="Y3" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="Z3" s="40" t="s">
+      <c r="Z3" s="37" t="s">
         <v>64</v>
       </c>
-      <c r="AA3" s="40" t="s">
+      <c r="AA3" s="37" t="s">
         <v>64</v>
       </c>
-      <c r="AB3" s="40" t="s">
+      <c r="AB3" s="37" t="s">
         <v>64</v>
       </c>
-      <c r="AC3" s="40" t="s">
+      <c r="AC3" s="37" t="s">
         <v>64</v>
       </c>
-      <c r="AD3" s="40" t="s">
+      <c r="AD3" s="37" t="s">
         <v>64</v>
       </c>
-      <c r="AE3" s="40" t="s">
+      <c r="AE3" s="37" t="s">
         <v>64</v>
       </c>
       <c r="AF3" s="24">
-        <f>COUNTIF(B3:AE3, "*x*")</f>
+        <f t="shared" si="0"/>
         <v>27</v>
       </c>
     </row>
@@ -4646,7 +4688,7 @@
       <c r="H4" s="28"/>
       <c r="I4" s="28"/>
       <c r="J4" s="7"/>
-      <c r="K4" s="40" t="s">
+      <c r="K4" s="37" t="s">
         <v>64</v>
       </c>
       <c r="L4" s="28"/>
@@ -4655,36 +4697,36 @@
       <c r="O4" s="28"/>
       <c r="P4" s="28"/>
       <c r="Q4" s="28"/>
-      <c r="R4" s="40" t="s">
+      <c r="R4" s="37" t="s">
         <v>64</v>
       </c>
       <c r="S4" s="15"/>
       <c r="T4" s="15"/>
-      <c r="U4" s="40" t="s">
+      <c r="U4" s="37" t="s">
         <v>64</v>
       </c>
-      <c r="V4" s="40" t="s">
+      <c r="V4" s="37" t="s">
         <v>64</v>
       </c>
-      <c r="W4" s="40" t="s">
+      <c r="W4" s="37" t="s">
         <v>64</v>
       </c>
       <c r="X4" s="25"/>
       <c r="Y4" s="7"/>
-      <c r="Z4" s="40" t="s">
+      <c r="Z4" s="37" t="s">
         <v>64</v>
       </c>
       <c r="AA4" s="7"/>
       <c r="AB4" s="7"/>
       <c r="AC4" s="7"/>
-      <c r="AD4" s="40" t="s">
+      <c r="AD4" s="37" t="s">
         <v>64</v>
       </c>
-      <c r="AE4" s="40" t="s">
+      <c r="AE4" s="37" t="s">
         <v>64</v>
       </c>
       <c r="AF4" s="24">
-        <f>COUNTIF(B4:AE4, "*x*")</f>
+        <f t="shared" si="0"/>
         <v>9</v>
       </c>
     </row>
@@ -4703,59 +4745,59 @@
         <v>64</v>
       </c>
       <c r="F5" s="7"/>
-      <c r="G5" s="40" t="s">
+      <c r="G5" s="37" t="s">
         <v>64</v>
       </c>
       <c r="H5" s="7"/>
       <c r="I5" s="7"/>
-      <c r="J5" s="40" t="s">
+      <c r="J5" s="37" t="s">
         <v>64</v>
       </c>
-      <c r="K5" s="40" t="s">
+      <c r="K5" s="37" t="s">
         <v>64</v>
       </c>
-      <c r="L5" s="40" t="s">
+      <c r="L5" s="37" t="s">
         <v>64</v>
       </c>
       <c r="M5" s="7"/>
       <c r="N5" s="7"/>
-      <c r="O5" s="40" t="s">
+      <c r="O5" s="37" t="s">
         <v>64</v>
       </c>
       <c r="P5" s="7"/>
-      <c r="Q5" s="40" t="s">
+      <c r="Q5" s="37" t="s">
         <v>64</v>
       </c>
-      <c r="R5" s="40" t="s">
+      <c r="R5" s="37" t="s">
         <v>64</v>
       </c>
-      <c r="S5" s="40" t="s">
+      <c r="S5" s="37" t="s">
         <v>64</v>
       </c>
-      <c r="T5" s="40" t="s">
+      <c r="T5" s="37" t="s">
         <v>64</v>
       </c>
-      <c r="U5" s="40" t="s">
+      <c r="U5" s="37" t="s">
         <v>64</v>
       </c>
       <c r="V5" s="15"/>
       <c r="W5" s="7"/>
-      <c r="X5" s="40" t="s">
+      <c r="X5" s="37" t="s">
         <v>64</v>
       </c>
       <c r="Y5" s="7"/>
       <c r="Z5" s="7"/>
-      <c r="AA5" s="40" t="s">
+      <c r="AA5" s="37" t="s">
         <v>64</v>
       </c>
       <c r="AB5" s="7"/>
-      <c r="AC5" s="40" t="s">
+      <c r="AC5" s="37" t="s">
         <v>64</v>
       </c>
       <c r="AD5" s="7"/>
       <c r="AE5" s="7"/>
       <c r="AF5" s="24">
-        <f>COUNTIF(B5:AE5, "*x*")</f>
+        <f t="shared" si="0"/>
         <v>16</v>
       </c>
     </row>
@@ -4776,79 +4818,79 @@
         <v>64</v>
       </c>
       <c r="F6" s="7"/>
-      <c r="G6" s="40" t="s">
+      <c r="G6" s="37" t="s">
         <v>64</v>
       </c>
-      <c r="H6" s="40" t="s">
+      <c r="H6" s="37" t="s">
         <v>64</v>
       </c>
-      <c r="I6" s="40" t="s">
+      <c r="I6" s="37" t="s">
         <v>64</v>
       </c>
-      <c r="J6" s="40" t="s">
+      <c r="J6" s="37" t="s">
         <v>64</v>
       </c>
-      <c r="K6" s="40" t="s">
+      <c r="K6" s="37" t="s">
         <v>64</v>
       </c>
-      <c r="L6" s="40" t="s">
+      <c r="L6" s="37" t="s">
         <v>64</v>
       </c>
-      <c r="M6" s="40" t="s">
+      <c r="M6" s="37" t="s">
         <v>64</v>
       </c>
-      <c r="N6" s="40" t="s">
+      <c r="N6" s="37" t="s">
         <v>64</v>
       </c>
-      <c r="O6" s="40" t="s">
+      <c r="O6" s="37" t="s">
         <v>64</v>
       </c>
-      <c r="P6" s="40" t="s">
+      <c r="P6" s="37" t="s">
         <v>64</v>
       </c>
-      <c r="Q6" s="40" t="s">
+      <c r="Q6" s="37" t="s">
         <v>64</v>
       </c>
-      <c r="R6" s="40" t="s">
+      <c r="R6" s="37" t="s">
         <v>64</v>
       </c>
-      <c r="S6" s="40" t="s">
+      <c r="S6" s="37" t="s">
         <v>64</v>
       </c>
-      <c r="T6" s="40" t="s">
+      <c r="T6" s="37" t="s">
         <v>64</v>
       </c>
-      <c r="U6" s="40" t="s">
+      <c r="U6" s="37" t="s">
         <v>64</v>
       </c>
-      <c r="V6" s="40" t="s">
+      <c r="V6" s="37" t="s">
         <v>64</v>
       </c>
       <c r="W6" s="7"/>
-      <c r="X6" s="40" t="s">
+      <c r="X6" s="37" t="s">
         <v>64</v>
       </c>
-      <c r="Y6" s="40" t="s">
+      <c r="Y6" s="37" t="s">
         <v>64</v>
       </c>
-      <c r="Z6" s="40" t="s">
+      <c r="Z6" s="37" t="s">
         <v>64</v>
       </c>
-      <c r="AA6" s="40" t="s">
+      <c r="AA6" s="37" t="s">
         <v>64</v>
       </c>
-      <c r="AB6" s="40" t="s">
+      <c r="AB6" s="37" t="s">
         <v>64</v>
       </c>
-      <c r="AC6" s="40" t="s">
+      <c r="AC6" s="37" t="s">
         <v>64</v>
       </c>
-      <c r="AD6" s="40" t="s">
+      <c r="AD6" s="37" t="s">
         <v>64</v>
       </c>
       <c r="AE6" s="7"/>
       <c r="AF6" s="24">
-        <f>COUNTIF(B6:AE6, "*x*")</f>
+        <f t="shared" si="0"/>
         <v>27</v>
       </c>
     </row>
@@ -4867,24 +4909,24 @@
       <c r="F7" s="7"/>
       <c r="G7" s="7"/>
       <c r="H7" s="7"/>
-      <c r="I7" s="40" t="s">
+      <c r="I7" s="37" t="s">
         <v>64</v>
       </c>
       <c r="J7" s="7"/>
       <c r="K7" s="7"/>
       <c r="L7" s="7"/>
       <c r="M7" s="7"/>
-      <c r="N7" s="40" t="s">
+      <c r="N7" s="37" t="s">
         <v>64</v>
       </c>
       <c r="O7" s="7"/>
-      <c r="P7" s="40" t="s">
+      <c r="P7" s="37" t="s">
         <v>64</v>
       </c>
       <c r="Q7" s="7"/>
       <c r="R7" s="15"/>
       <c r="S7" s="15"/>
-      <c r="T7" s="40" t="s">
+      <c r="T7" s="37" t="s">
         <v>64</v>
       </c>
       <c r="U7" s="15"/>
@@ -4895,13 +4937,13 @@
       <c r="Z7" s="7"/>
       <c r="AA7" s="7"/>
       <c r="AB7" s="7"/>
-      <c r="AC7" s="40" t="s">
+      <c r="AC7" s="37" t="s">
         <v>64</v>
       </c>
       <c r="AD7" s="7"/>
       <c r="AE7" s="7"/>
       <c r="AF7" s="24">
-        <f>COUNTIF(B7:AE7, "*x*")</f>
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
     </row>
@@ -4921,7 +4963,7 @@
       <c r="K8" s="15"/>
       <c r="L8" s="15"/>
       <c r="M8" s="15"/>
-      <c r="N8" s="40" t="s">
+      <c r="N8" s="37" t="s">
         <v>64</v>
       </c>
       <c r="O8" s="15"/>
@@ -4931,14 +4973,14 @@
       <c r="S8" s="7"/>
       <c r="T8" s="7"/>
       <c r="U8" s="7"/>
-      <c r="V8" s="40" t="s">
+      <c r="V8" s="37" t="s">
         <v>64</v>
       </c>
-      <c r="W8" s="40" t="s">
+      <c r="W8" s="37" t="s">
         <v>64</v>
       </c>
       <c r="X8" s="7"/>
-      <c r="Y8" s="40" t="s">
+      <c r="Y8" s="37" t="s">
         <v>64</v>
       </c>
       <c r="Z8" s="7"/>
@@ -4948,7 +4990,7 @@
       <c r="AD8" s="7"/>
       <c r="AE8" s="7"/>
       <c r="AF8" s="24">
-        <f>COUNTIF(B8:AE8, "*x*")</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
     </row>
@@ -5113,10 +5155,10 @@
       </c>
     </row>
     <row r="2" spans="1:34" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="37" t="s">
+      <c r="A2" s="38" t="s">
         <v>55</v>
       </c>
-      <c r="B2" s="38" t="s">
+      <c r="B2" s="39" t="s">
         <v>56</v>
       </c>
       <c r="C2" s="15" t="s">
@@ -5149,14 +5191,14 @@
       <c r="V2" s="15"/>
       <c r="W2" s="15"/>
       <c r="X2" s="15"/>
-      <c r="AH2" s="39">
+      <c r="AH2" s="40">
         <f>COUNTIF(D2:AG3, "*x*")</f>
         <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:34" ht="13.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="37"/>
-      <c r="B3" s="38"/>
+      <c r="A3" s="38"/>
+      <c r="B3" s="39"/>
       <c r="C3" s="15" t="s">
         <v>59</v>
       </c>
@@ -5184,13 +5226,13 @@
       <c r="AA3" s="26" t="s">
         <v>60</v>
       </c>
-      <c r="AH3" s="39"/>
+      <c r="AH3" s="40"/>
     </row>
     <row r="4" spans="1:34" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="37" t="s">
+      <c r="A4" s="38" t="s">
         <v>61</v>
       </c>
-      <c r="B4" s="38" t="s">
+      <c r="B4" s="39" t="s">
         <v>62</v>
       </c>
       <c r="C4" s="15" t="s">
@@ -5265,14 +5307,14 @@
         <v>69</v>
       </c>
       <c r="AG4" s="15"/>
-      <c r="AH4" s="39">
+      <c r="AH4" s="40">
         <f>COUNTIF(D4:AG5, "*x*")</f>
         <v>45</v>
       </c>
     </row>
     <row r="5" spans="1:34" ht="12.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="37"/>
-      <c r="B5" s="38"/>
+      <c r="A5" s="38"/>
+      <c r="B5" s="39"/>
       <c r="C5" s="15" t="s">
         <v>70</v>
       </c>
@@ -5355,7 +5397,7 @@
       <c r="AG5" s="15" t="s">
         <v>64</v>
       </c>
-      <c r="AH5" s="39"/>
+      <c r="AH5" s="40"/>
     </row>
     <row r="6" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="27" t="s">
@@ -5634,10 +5676,10 @@
       </c>
     </row>
     <row r="10" spans="1:34" ht="13.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="37" t="s">
+      <c r="A10" s="38" t="s">
         <v>95</v>
       </c>
-      <c r="B10" s="38" t="s">
+      <c r="B10" s="39" t="s">
         <v>96</v>
       </c>
       <c r="C10" s="15" t="s">
@@ -5675,14 +5717,14 @@
       <c r="AA10" s="26" t="s">
         <v>99</v>
       </c>
-      <c r="AH10" s="39">
+      <c r="AH10" s="40">
         <f>COUNTIF(D10:AG11, "*x*")</f>
         <v>6</v>
       </c>
     </row>
     <row r="11" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="37"/>
-      <c r="B11" s="38"/>
+      <c r="A11" s="38"/>
+      <c r="B11" s="39"/>
       <c r="C11" s="15" t="s">
         <v>100</v>
       </c>
@@ -5713,7 +5755,7 @@
       </c>
       <c r="Y11" s="7"/>
       <c r="Z11" s="7"/>
-      <c r="AH11" s="39"/>
+      <c r="AH11" s="40"/>
     </row>
     <row r="12" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A12" s="27"/>

</xml_diff>